<commit_message>
Original Code for Policy
Policy
</commit_message>
<xml_diff>
--- a/Eclipse/Week1/Datafiles/Insurance.xlsx
+++ b/Eclipse/Week1/Datafiles/Insurance.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>leo</t>
+  </si>
+  <si>
+    <t>alexandra</t>
   </si>
 </sst>
 </file>
@@ -644,16 +647,25 @@
         <v>33</v>
       </c>
       <c r="B14" t="n" s="0">
-        <v>29.0</v>
+        <v>78.0</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>486.0</v>
+        <v>722.0</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B15" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>486.0</v>
+      </c>
       <c r="D15" t="s" s="0">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
12/11/24 All College Files
</commit_message>
<xml_diff>
--- a/Eclipse/Week1/Datafiles/Insurance.xlsx
+++ b/Eclipse/Week1/Datafiles/Insurance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fowle\Desktop\CollegeGit\Eclipse\Week1\Datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E5AAA9-C786-4B34-927C-DE91C130D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6663DD00-AB70-400D-9E99-6831EFC21588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="340" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>alexandra</t>
+  </si>
+  <si>
+    <t>scottie</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>billybob</t>
+  </si>
+  <si>
+    <t>bobbert</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,10 +491,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>29.0</v>
+        <v>24.0</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>486.0</v>
+        <v>406.0</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>13</v>
@@ -605,10 +617,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="0">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C11" s="0">
-        <v>486</v>
+        <v>406</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>22</v>
@@ -618,11 +630,11 @@
       <c r="A12" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B12" t="n" s="0">
-        <v>29.0</v>
-      </c>
-      <c r="C12" t="n" s="0">
-        <v>486.0</v>
+      <c r="B12" s="0">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0">
+        <v>486</v>
       </c>
       <c r="D12" t="s" s="0">
         <v>23</v>
@@ -632,11 +644,11 @@
       <c r="A13" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B13" t="n" s="0">
-        <v>39.0</v>
-      </c>
-      <c r="C13" t="n" s="0">
-        <v>722.0</v>
+      <c r="B13" s="0">
+        <v>39</v>
+      </c>
+      <c r="C13" s="0">
+        <v>722</v>
       </c>
       <c r="D13" t="s" s="0">
         <v>24</v>
@@ -646,11 +658,11 @@
       <c r="A14" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B14" t="n" s="0">
-        <v>78.0</v>
-      </c>
-      <c r="C14" t="n" s="0">
-        <v>722.0</v>
+      <c r="B14" s="0">
+        <v>78</v>
+      </c>
+      <c r="C14" s="0">
+        <v>722</v>
       </c>
       <c r="D14" t="s" s="0">
         <v>25</v>
@@ -660,30 +672,63 @@
       <c r="A15" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B15" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>486.0</v>
+      <c r="B15" s="0">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0">
+        <v>486</v>
       </c>
       <c r="D15" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B16" s="0">
+        <v>26</v>
+      </c>
+      <c r="C16" s="0">
+        <v>406</v>
+      </c>
       <c r="D16" t="s" s="0">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B17" s="0">
+        <v>28</v>
+      </c>
+      <c r="C17" s="0">
+        <v>470</v>
+      </c>
       <c r="D17" t="s" s="0">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B18" s="0">
+        <v>12</v>
+      </c>
       <c r="D18" t="s" s="0">
         <v>29</v>
       </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B19" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="C19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>